<commit_message>
Add SHT inventory with adapter model/slot
Signed-off-by: Dung K Hoang <DungKHoang@gmail.com>
</commit_message>
<xml_diff>
--- a/OV-Template.xlsx
+++ b/OV-Template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-Temp\Import-Export-OneView-Resources-9\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00017552-45BE-4650-887C-81D0FA1285C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED5A3675-EE43-49D1-B6D3-F417E21D7D4A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="28" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="28" activeTab="30" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Version" sheetId="11" r:id="rId1"/>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1196" uniqueCount="709">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="713">
   <si>
     <t>#Configure Logical InterConnect Group</t>
   </si>
@@ -4056,6 +4056,18 @@
   </si>
   <si>
     <t>formFactor</t>
+  </si>
+  <si>
+    <t>adapterModel</t>
+  </si>
+  <si>
+    <t>adapterSlot</t>
+  </si>
+  <si>
+    <t># List of adapter model separated by '|'</t>
+  </si>
+  <si>
+    <t># List of adapter slot separated by '|'</t>
   </si>
 </sst>
 </file>
@@ -13174,15 +13186,16 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B14" sqref="B14"/>
+      <selection pane="bottomLeft" activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.7109375" style="4" customWidth="1"/>
     <col min="2" max="3" width="35.85546875" style="4" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" style="4" customWidth="1"/>
-    <col min="5" max="7" width="23.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="41.140625" style="4" customWidth="1"/>
+    <col min="5" max="5" width="35.140625" style="4" customWidth="1"/>
+    <col min="6" max="7" width="23.140625" style="4" customWidth="1"/>
     <col min="8" max="8" width="30.7109375" style="4" customWidth="1"/>
     <col min="9" max="9" width="23.140625" style="4" customWidth="1"/>
     <col min="10" max="10" width="31.140625" style="4" customWidth="1"/>
@@ -13210,13 +13223,17 @@
         <v>64</v>
       </c>
       <c r="B1" s="38" t="s">
+        <v>434</v>
+      </c>
+      <c r="C1" s="38" t="s">
         <v>708</v>
       </c>
-      <c r="C1" s="38" t="s">
-        <v>434</v>
-      </c>
-      <c r="D1" s="124"/>
-      <c r="E1" s="5"/>
+      <c r="D1" s="124" t="s">
+        <v>709</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>710</v>
+      </c>
       <c r="F1" s="5"/>
       <c r="G1" s="125"/>
       <c r="H1" s="125"/>
@@ -13325,8 +13342,12 @@
       </c>
       <c r="B7" s="135"/>
       <c r="C7" s="135"/>
-      <c r="D7" s="135"/>
-      <c r="E7" s="136"/>
+      <c r="D7" s="135" t="s">
+        <v>711</v>
+      </c>
+      <c r="E7" s="135" t="s">
+        <v>712</v>
+      </c>
       <c r="F7" s="136"/>
       <c r="G7" s="136"/>
       <c r="H7" s="137"/>
@@ -20888,12 +20909,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B306D734CEBD84FBBC41786449802E3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="16005ef843dd214786fd86ac676497e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="54a4fa2c-6341-4596-b8d8-a2e023346efc" xmlns:ns4="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2325c866b17d621340695414d4ca9b0e" ns3:_="" ns4:_="">
     <xsd:import namespace="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
@@ -21110,6 +21125,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -21120,23 +21141,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7124AFE1-C9C5-46E7-A048-9DDD62293557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21155,6 +21159,23 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Fix Issue #6: Array of target - OV-Template
Signed-off-by: Dung K Hoang <DungKHoang@gmail.com>
</commit_message>
<xml_diff>
--- a/OV-Template.xlsx
+++ b/OV-Template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-Temp\Import-Export-OneView-Resources-11\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Github-Temp\Import-Export-OneView-Resources-13\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{472432EC-306B-47D5-8759-7B5DF543719D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75964978-0458-4C3D-9268-9171E19782C9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="723" firstSheet="31" activeTab="37" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -74,7 +74,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1204" uniqueCount="717">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="715">
   <si>
     <t>#Configure Logical InterConnect Group</t>
   </si>
@@ -4066,20 +4066,6 @@
     <t># List of adapter slot separated by '|'</t>
   </si>
   <si>
-    <t>bootTarget</t>
-  </si>
-  <si>
-    <t>targetLUN</t>
-  </si>
-  <si>
-    <t># if bootVolumeSource = 'userDefined'
-#Specify WWPN of target LUN</t>
-  </si>
-  <si>
-    <t xml:space="preserve"># if bootVolumeSource = 'userDefined'
-# Specify lunID of target LUN </t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve"># By default userDefined = FALSE
 # If you want to use custom MAC/WWPN/WWNN specified in the right columns, you need to set it to TRUE. We will then , we will create a connection with custom MAC and WWN
@@ -4106,6 +4092,14 @@
       </rPr>
       <t xml:space="preserve"> configuration. Administrator needs to explicitly set it for the import  operation and apply for server profile only!</t>
     </r>
+  </si>
+  <si>
+    <t>targets</t>
+  </si>
+  <si>
+    <t># if bootVolumeSource = 'userDefined'
+#Specify an array of hash:
+# {targetWWPN, Lun}</t>
   </si>
 </sst>
 </file>
@@ -17868,11 +17862,11 @@
 
 <file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5476BCB0-492A-4349-9B4C-02D8DB45D26B}">
-  <dimension ref="A1:V79"/>
+  <dimension ref="A1:U79"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="H1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M8" sqref="M8"/>
+      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -17887,18 +17881,17 @@
     <col min="9" max="9" width="33.140625" style="4" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" style="4" customWidth="1"/>
     <col min="11" max="11" width="24.5703125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="22.7109375" style="4" customWidth="1"/>
-    <col min="13" max="13" width="33.140625" style="4" customWidth="1"/>
-    <col min="14" max="15" width="23.42578125" customWidth="1"/>
-    <col min="16" max="16" width="23" customWidth="1"/>
-    <col min="17" max="17" width="18.42578125" customWidth="1"/>
-    <col min="18" max="18" width="18.42578125" style="4" customWidth="1"/>
-    <col min="19" max="19" width="18" style="4" customWidth="1"/>
-    <col min="20" max="20" width="21.42578125" customWidth="1"/>
-    <col min="21" max="21" width="21" customWidth="1"/>
+    <col min="12" max="12" width="33.140625" style="4" customWidth="1"/>
+    <col min="13" max="14" width="23.42578125" customWidth="1"/>
+    <col min="15" max="15" width="23" customWidth="1"/>
+    <col min="16" max="16" width="18.42578125" customWidth="1"/>
+    <col min="17" max="17" width="18.42578125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="18" style="4" customWidth="1"/>
+    <col min="19" max="19" width="21.42578125" customWidth="1"/>
+    <col min="20" max="20" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="38" t="s">
         <v>145</v>
       </c>
@@ -17930,43 +17923,40 @@
         <v>691</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>712</v>
+        <v>713</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>713</v>
-      </c>
-      <c r="M1" s="5" t="s">
         <v>205</v>
       </c>
-      <c r="N1" s="111" t="s">
+      <c r="M1" s="111" t="s">
         <v>129</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>206</v>
       </c>
-      <c r="P1" s="111" t="s">
+      <c r="O1" s="111" t="s">
         <v>324</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="R1" s="5" t="s">
+      <c r="Q1" s="5" t="s">
         <v>208</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>209</v>
       </c>
+      <c r="S1" s="5" t="s">
+        <v>233</v>
+      </c>
       <c r="T1" s="5" t="s">
-        <v>233</v>
-      </c>
-      <c r="U1" s="5" t="s">
         <v>687</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>688</v>
       </c>
     </row>
-    <row r="2" spans="1:22" s="20" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" s="20" customFormat="1" ht="18" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>238</v>
       </c>
@@ -17977,9 +17967,8 @@
       <c r="J2" s="34"/>
       <c r="K2" s="34"/>
       <c r="L2" s="34"/>
-      <c r="M2" s="34"/>
-    </row>
-    <row r="3" spans="1:22" s="17" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:21" s="17" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
         <v>6</v>
       </c>
@@ -17989,9 +17978,8 @@
       <c r="J3" s="23"/>
       <c r="K3" s="23"/>
       <c r="L3" s="23"/>
-      <c r="M3" s="23"/>
-    </row>
-    <row r="4" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
         <v>8</v>
       </c>
@@ -18001,9 +17989,8 @@
       <c r="J4" s="23"/>
       <c r="K4" s="23"/>
       <c r="L4" s="23"/>
-      <c r="M4" s="23"/>
-    </row>
-    <row r="5" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="57" t="s">
         <v>38</v>
       </c>
@@ -18013,9 +18000,8 @@
       <c r="J5" s="23"/>
       <c r="K5" s="23"/>
       <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-    </row>
-    <row r="6" spans="1:22" s="17" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:21" s="17" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
         <v>14</v>
       </c>
@@ -18026,12 +18012,11 @@
       <c r="K6" s="23"/>
       <c r="L6" s="23"/>
       <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
+      <c r="R6" s="23"/>
       <c r="S6" s="23"/>
       <c r="T6" s="23"/>
-      <c r="U6" s="23"/>
-    </row>
-    <row r="7" spans="1:22" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22"/>
       <c r="B7" s="19"/>
       <c r="C7" s="19"/>
@@ -18046,12 +18031,11 @@
       <c r="M7" s="19"/>
       <c r="N7" s="19"/>
       <c r="O7" s="19"/>
-      <c r="P7" s="19"/>
+      <c r="R7" s="19"/>
       <c r="S7" s="19"/>
       <c r="T7" s="19"/>
-      <c r="U7" s="19"/>
-    </row>
-    <row r="8" spans="1:22" s="82" customFormat="1" ht="193.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:21" s="82" customFormat="1" ht="193.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="42" t="s">
         <v>39</v>
       </c>
@@ -18086,38 +18070,35 @@
         <v>714</v>
       </c>
       <c r="L8" s="50" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="M8" s="50" t="s">
-        <v>716</v>
-      </c>
-      <c r="N8" s="50" t="s">
         <v>212</v>
       </c>
-      <c r="O8" s="41" t="s">
+      <c r="N8" s="41" t="s">
         <v>45</v>
       </c>
-      <c r="P8" s="50" t="s">
+      <c r="O8" s="50" t="s">
         <v>212</v>
       </c>
+      <c r="P8" s="41" t="s">
+        <v>46</v>
+      </c>
       <c r="Q8" s="41" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="R8" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="S8" s="41" t="s">
         <v>211</v>
       </c>
-      <c r="T8" s="42" t="s">
+      <c r="S8" s="42" t="s">
         <v>234</v>
       </c>
-      <c r="U8" s="49" t="s">
+      <c r="T8" s="49" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="9" spans="1:22" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11"/>
       <c r="B11"/>
       <c r="D11"/>
@@ -18126,9 +18107,8 @@
       <c r="H11"/>
       <c r="J11"/>
       <c r="K11"/>
-      <c r="L11"/>
-    </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12"/>
       <c r="B12"/>
       <c r="D12"/>
@@ -18137,9 +18117,8 @@
       <c r="H12"/>
       <c r="J12"/>
       <c r="K12"/>
-      <c r="L12"/>
-    </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13"/>
       <c r="B13"/>
       <c r="D13"/>
@@ -18148,9 +18127,8 @@
       <c r="H13"/>
       <c r="J13"/>
       <c r="K13"/>
-      <c r="L13"/>
-    </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14"/>
       <c r="B14"/>
       <c r="D14"/>
@@ -18159,9 +18137,8 @@
       <c r="H14"/>
       <c r="J14"/>
       <c r="K14"/>
-      <c r="L14"/>
-    </row>
-    <row r="15" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15"/>
       <c r="B15"/>
       <c r="D15"/>
@@ -18170,9 +18147,8 @@
       <c r="H15"/>
       <c r="J15"/>
       <c r="K15"/>
-      <c r="L15"/>
-    </row>
-    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16"/>
       <c r="B16"/>
       <c r="D16"/>
@@ -18181,9 +18157,8 @@
       <c r="H16"/>
       <c r="J16"/>
       <c r="K16"/>
-      <c r="L16"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17"/>
       <c r="B17"/>
       <c r="D17"/>
@@ -18192,9 +18167,8 @@
       <c r="H17"/>
       <c r="J17"/>
       <c r="K17"/>
-      <c r="L17"/>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18"/>
       <c r="B18"/>
       <c r="D18"/>
@@ -18203,9 +18177,8 @@
       <c r="H18"/>
       <c r="J18"/>
       <c r="K18"/>
-      <c r="L18"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19"/>
       <c r="B19"/>
       <c r="D19"/>
@@ -18214,9 +18187,8 @@
       <c r="H19"/>
       <c r="J19"/>
       <c r="K19"/>
-      <c r="L19"/>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20"/>
       <c r="B20"/>
       <c r="D20"/>
@@ -18225,9 +18197,8 @@
       <c r="H20"/>
       <c r="J20"/>
       <c r="K20"/>
-      <c r="L20"/>
-    </row>
-    <row r="21" spans="1:12" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:11" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21"/>
       <c r="B21"/>
       <c r="D21"/>
@@ -18236,9 +18207,8 @@
       <c r="H21"/>
       <c r="J21"/>
       <c r="K21"/>
-      <c r="L21"/>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22"/>
       <c r="B22"/>
       <c r="D22"/>
@@ -18247,9 +18217,8 @@
       <c r="H22"/>
       <c r="J22"/>
       <c r="K22"/>
-      <c r="L22"/>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23"/>
       <c r="B23"/>
       <c r="D23"/>
@@ -18258,9 +18227,8 @@
       <c r="H23"/>
       <c r="J23"/>
       <c r="K23"/>
-      <c r="L23"/>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24"/>
       <c r="B24"/>
       <c r="D24"/>
@@ -18269,9 +18237,8 @@
       <c r="H24"/>
       <c r="J24"/>
       <c r="K24"/>
-      <c r="L24"/>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25"/>
       <c r="B25"/>
       <c r="D25"/>
@@ -18280,9 +18247,8 @@
       <c r="H25"/>
       <c r="J25"/>
       <c r="K25"/>
-      <c r="L25"/>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26"/>
       <c r="B26"/>
       <c r="D26"/>
@@ -18291,9 +18257,8 @@
       <c r="H26"/>
       <c r="J26"/>
       <c r="K26"/>
-      <c r="L26"/>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27"/>
       <c r="B27"/>
       <c r="D27"/>
@@ -18302,9 +18267,8 @@
       <c r="H27"/>
       <c r="J27"/>
       <c r="K27"/>
-      <c r="L27"/>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28"/>
       <c r="B28"/>
       <c r="D28"/>
@@ -18313,9 +18277,8 @@
       <c r="H28"/>
       <c r="J28"/>
       <c r="K28"/>
-      <c r="L28"/>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29"/>
       <c r="B29"/>
       <c r="D29"/>
@@ -18324,9 +18287,8 @@
       <c r="H29"/>
       <c r="J29"/>
       <c r="K29"/>
-      <c r="L29"/>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30"/>
       <c r="B30"/>
       <c r="D30"/>
@@ -18335,9 +18297,8 @@
       <c r="H30"/>
       <c r="J30"/>
       <c r="K30"/>
-      <c r="L30"/>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31"/>
       <c r="B31"/>
       <c r="D31"/>
@@ -18346,9 +18307,8 @@
       <c r="H31"/>
       <c r="J31"/>
       <c r="K31"/>
-      <c r="L31"/>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32"/>
       <c r="B32"/>
       <c r="D32"/>
@@ -18357,9 +18317,8 @@
       <c r="H32"/>
       <c r="J32"/>
       <c r="K32"/>
-      <c r="L32"/>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33"/>
       <c r="B33"/>
       <c r="D33"/>
@@ -18368,9 +18327,8 @@
       <c r="H33"/>
       <c r="J33"/>
       <c r="K33"/>
-      <c r="L33"/>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34"/>
       <c r="B34"/>
       <c r="D34"/>
@@ -18379,9 +18337,8 @@
       <c r="H34"/>
       <c r="J34"/>
       <c r="K34"/>
-      <c r="L34"/>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35"/>
       <c r="B35"/>
       <c r="D35"/>
@@ -18390,9 +18347,8 @@
       <c r="H35"/>
       <c r="J35"/>
       <c r="K35"/>
-      <c r="L35"/>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36"/>
       <c r="B36"/>
       <c r="D36"/>
@@ -18401,9 +18357,8 @@
       <c r="H36"/>
       <c r="J36"/>
       <c r="K36"/>
-      <c r="L36"/>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37"/>
       <c r="B37"/>
       <c r="D37"/>
@@ -18412,9 +18367,8 @@
       <c r="H37"/>
       <c r="J37"/>
       <c r="K37"/>
-      <c r="L37"/>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38"/>
       <c r="B38"/>
       <c r="D38"/>
@@ -18423,9 +18377,8 @@
       <c r="H38"/>
       <c r="J38"/>
       <c r="K38"/>
-      <c r="L38"/>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39"/>
       <c r="B39"/>
       <c r="D39"/>
@@ -18434,9 +18387,8 @@
       <c r="H39"/>
       <c r="J39"/>
       <c r="K39"/>
-      <c r="L39"/>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40"/>
       <c r="B40"/>
       <c r="D40"/>
@@ -18445,9 +18397,8 @@
       <c r="H40"/>
       <c r="J40"/>
       <c r="K40"/>
-      <c r="L40"/>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41"/>
       <c r="B41"/>
       <c r="D41"/>
@@ -18456,9 +18407,8 @@
       <c r="H41"/>
       <c r="J41"/>
       <c r="K41"/>
-      <c r="L41"/>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42"/>
       <c r="B42"/>
       <c r="D42"/>
@@ -18467,9 +18417,8 @@
       <c r="H42"/>
       <c r="J42"/>
       <c r="K42"/>
-      <c r="L42"/>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43"/>
       <c r="B43"/>
       <c r="D43"/>
@@ -18478,9 +18427,8 @@
       <c r="H43"/>
       <c r="J43"/>
       <c r="K43"/>
-      <c r="L43"/>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44"/>
       <c r="B44"/>
       <c r="D44"/>
@@ -18489,9 +18437,8 @@
       <c r="H44"/>
       <c r="J44"/>
       <c r="K44"/>
-      <c r="L44"/>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45"/>
       <c r="B45"/>
       <c r="D45"/>
@@ -18500,9 +18447,8 @@
       <c r="H45"/>
       <c r="J45"/>
       <c r="K45"/>
-      <c r="L45"/>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46"/>
       <c r="B46"/>
       <c r="D46"/>
@@ -18511,9 +18457,8 @@
       <c r="H46"/>
       <c r="J46"/>
       <c r="K46"/>
-      <c r="L46"/>
-    </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47"/>
       <c r="B47"/>
       <c r="D47"/>
@@ -18522,9 +18467,8 @@
       <c r="H47"/>
       <c r="J47"/>
       <c r="K47"/>
-      <c r="L47"/>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48"/>
       <c r="B48"/>
       <c r="D48"/>
@@ -18533,9 +18477,8 @@
       <c r="H48"/>
       <c r="J48"/>
       <c r="K48"/>
-      <c r="L48"/>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49"/>
       <c r="B49"/>
       <c r="D49"/>
@@ -18544,9 +18487,8 @@
       <c r="H49"/>
       <c r="J49"/>
       <c r="K49"/>
-      <c r="L49"/>
-    </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50"/>
       <c r="B50"/>
       <c r="D50"/>
@@ -18555,9 +18497,8 @@
       <c r="H50"/>
       <c r="J50"/>
       <c r="K50"/>
-      <c r="L50"/>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51"/>
       <c r="B51"/>
       <c r="D51"/>
@@ -18566,9 +18507,8 @@
       <c r="H51"/>
       <c r="J51"/>
       <c r="K51"/>
-      <c r="L51"/>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A52"/>
       <c r="B52"/>
       <c r="D52"/>
@@ -18577,9 +18517,8 @@
       <c r="H52"/>
       <c r="J52"/>
       <c r="K52"/>
-      <c r="L52"/>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A53"/>
       <c r="B53"/>
       <c r="D53"/>
@@ -18588,9 +18527,8 @@
       <c r="H53"/>
       <c r="J53"/>
       <c r="K53"/>
-      <c r="L53"/>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A54"/>
       <c r="B54"/>
       <c r="D54"/>
@@ -18599,9 +18537,8 @@
       <c r="H54"/>
       <c r="J54"/>
       <c r="K54"/>
-      <c r="L54"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A55"/>
       <c r="B55"/>
       <c r="D55"/>
@@ -18610,9 +18547,8 @@
       <c r="H55"/>
       <c r="J55"/>
       <c r="K55"/>
-      <c r="L55"/>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A56"/>
       <c r="B56"/>
       <c r="D56"/>
@@ -18621,9 +18557,8 @@
       <c r="H56"/>
       <c r="J56"/>
       <c r="K56"/>
-      <c r="L56"/>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A57"/>
       <c r="B57"/>
       <c r="D57"/>
@@ -18632,9 +18567,8 @@
       <c r="H57"/>
       <c r="J57"/>
       <c r="K57"/>
-      <c r="L57"/>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58"/>
       <c r="B58"/>
       <c r="D58"/>
@@ -18643,9 +18577,8 @@
       <c r="H58"/>
       <c r="J58"/>
       <c r="K58"/>
-      <c r="L58"/>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A59"/>
       <c r="B59"/>
       <c r="D59"/>
@@ -18654,9 +18587,8 @@
       <c r="H59"/>
       <c r="J59"/>
       <c r="K59"/>
-      <c r="L59"/>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A60"/>
       <c r="B60"/>
       <c r="D60"/>
@@ -18665,9 +18597,8 @@
       <c r="H60"/>
       <c r="J60"/>
       <c r="K60"/>
-      <c r="L60"/>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A61"/>
       <c r="B61"/>
       <c r="D61"/>
@@ -18676,9 +18607,8 @@
       <c r="H61"/>
       <c r="J61"/>
       <c r="K61"/>
-      <c r="L61"/>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A62"/>
       <c r="B62"/>
       <c r="D62"/>
@@ -18687,9 +18617,8 @@
       <c r="H62"/>
       <c r="J62"/>
       <c r="K62"/>
-      <c r="L62"/>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A63"/>
       <c r="B63"/>
       <c r="D63"/>
@@ -18698,9 +18627,8 @@
       <c r="H63"/>
       <c r="J63"/>
       <c r="K63"/>
-      <c r="L63"/>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A64"/>
       <c r="B64"/>
       <c r="D64"/>
@@ -18709,9 +18637,8 @@
       <c r="H64"/>
       <c r="J64"/>
       <c r="K64"/>
-      <c r="L64"/>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65"/>
       <c r="B65"/>
       <c r="D65"/>
@@ -18720,9 +18647,8 @@
       <c r="H65"/>
       <c r="J65"/>
       <c r="K65"/>
-      <c r="L65"/>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A66"/>
       <c r="B66"/>
       <c r="D66"/>
@@ -18731,9 +18657,8 @@
       <c r="H66"/>
       <c r="J66"/>
       <c r="K66"/>
-      <c r="L66"/>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A67"/>
       <c r="B67"/>
       <c r="D67"/>
@@ -18742,9 +18667,8 @@
       <c r="H67"/>
       <c r="J67"/>
       <c r="K67"/>
-      <c r="L67"/>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A68"/>
       <c r="B68"/>
       <c r="D68"/>
@@ -18753,9 +18677,8 @@
       <c r="H68"/>
       <c r="J68"/>
       <c r="K68"/>
-      <c r="L68"/>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>121</v>
       </c>
@@ -18766,9 +18689,8 @@
       <c r="H69"/>
       <c r="J69"/>
       <c r="K69"/>
-      <c r="L69"/>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A70"/>
       <c r="B70"/>
       <c r="D70"/>
@@ -18777,9 +18699,8 @@
       <c r="H70"/>
       <c r="J70"/>
       <c r="K70"/>
-      <c r="L70"/>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71"/>
       <c r="D71"/>
@@ -18788,9 +18709,8 @@
       <c r="H71"/>
       <c r="J71"/>
       <c r="K71"/>
-      <c r="L71"/>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72"/>
       <c r="D72"/>
@@ -18799,9 +18719,8 @@
       <c r="H72"/>
       <c r="J72"/>
       <c r="K72"/>
-      <c r="L72"/>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A73"/>
       <c r="B73"/>
       <c r="D73"/>
@@ -18810,9 +18729,8 @@
       <c r="H73"/>
       <c r="J73"/>
       <c r="K73"/>
-      <c r="L73"/>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A74"/>
       <c r="B74"/>
       <c r="D74"/>
@@ -18821,9 +18739,8 @@
       <c r="H74"/>
       <c r="J74"/>
       <c r="K74"/>
-      <c r="L74"/>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A75"/>
       <c r="B75"/>
       <c r="D75"/>
@@ -18832,9 +18749,8 @@
       <c r="H75"/>
       <c r="J75"/>
       <c r="K75"/>
-      <c r="L75"/>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A76"/>
       <c r="B76"/>
       <c r="D76"/>
@@ -18843,9 +18759,8 @@
       <c r="H76"/>
       <c r="J76"/>
       <c r="K76"/>
-      <c r="L76"/>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A77"/>
       <c r="B77"/>
       <c r="D77"/>
@@ -18854,9 +18769,8 @@
       <c r="H77"/>
       <c r="J77"/>
       <c r="K77"/>
-      <c r="L77"/>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A78"/>
       <c r="B78"/>
       <c r="D78"/>
@@ -18865,9 +18779,8 @@
       <c r="H78"/>
       <c r="J78"/>
       <c r="K78"/>
-      <c r="L78"/>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    </row>
+    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="D79"/>
     </row>
   </sheetData>
@@ -21123,15 +21036,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101008B306D734CEBD84FBBC41786449802E3" ma:contentTypeVersion="12" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="16005ef843dd214786fd86ac676497e8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="54a4fa2c-6341-4596-b8d8-a2e023346efc" xmlns:ns4="f7c671b8-1a97-4c58-b6a9-b872d1c47c8e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2325c866b17d621340695414d4ca9b0e" ns3:_="" ns4:_="">
     <xsd:import namespace="54a4fa2c-6341-4596-b8d8-a2e023346efc"/>
@@ -21348,6 +21252,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{43ECCFC7-29C2-4C1C-BA35-7A8B581B0FD8}">
   <ds:schemaRefs>
@@ -21366,14 +21279,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7124AFE1-C9C5-46E7-A048-9DDD62293557}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -21390,4 +21295,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B08671FF-7385-4DFE-A0B1-F772E0CBF546}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>